<commit_message>
[fix] fix end point of API
</commit_message>
<xml_diff>
--- a/20.開発/60.API/10.API一覧/API一覧.xlsx
+++ b/20.開発/60.API/10.API一覧/API一覧.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eternal\documents\20.開発\60.API\10.API一覧\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964D518C-6656-4DD0-886D-0D277E9AEFA0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B1FE78-E4EB-4CAF-9EB6-522F03376880}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="465" windowWidth="38400" windowHeight="21135" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
     <definedName name="改訂日">変更履歴!$D$5:$D$25</definedName>
     <definedName name="版">変更履歴!$B$5:$B$25</definedName>
   </definedNames>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
   <si>
     <t>API一覧</t>
     <rPh sb="3" eb="5">
@@ -200,18 +200,7 @@
     <t>hiima/api/internal/v1/talklist</t>
   </si>
   <si>
-    <t>hiima/api/internal/v1/commentlist</t>
-  </si>
-  <si>
-    <t>hiima/api/internal/v1/posttalk</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>hiima/api/internal/v1/evaluate</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>hiima/api/internal/v1/postcomment</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -324,10 +313,6 @@
     <rPh sb="4" eb="6">
       <t>ガメン</t>
     </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Ref005</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -555,6 +540,26 @@
     <rPh sb="31" eb="33">
       <t>ヘンコウ</t>
     </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Ref004</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>hiima/api/internal/v1/talkList</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>hiima/api/internal/v1/commentList</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>hiima/api/internal/v1/postTalk</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>hiima/api/internal/v1/postComment</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -836,26 +841,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1149,10 +1154,10 @@
   <sheetFormatPr defaultColWidth="7.6640625" defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="1.44140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="68.33203125" style="27" customWidth="1"/>
-    <col min="4" max="4" width="15" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="25" customWidth="1"/>
+    <col min="3" max="3" width="68.33203125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="15" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="25" customWidth="1"/>
     <col min="6" max="6" width="1.44140625" style="4" customWidth="1"/>
     <col min="7" max="16384" width="7.6640625" style="4"/>
   </cols>
@@ -1165,7 +1170,7 @@
     </row>
     <row r="2" spans="2:5">
       <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1179,175 +1184,175 @@
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="5" t="s">
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="C5" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="D5" s="23">
+        <v>43408</v>
+      </c>
+      <c r="E5" s="24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="25">
-        <v>43408</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>36</v>
-      </c>
-    </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="24" t="s">
+      <c r="B6" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="23">
+        <v>43434</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="25">
-        <v>43434</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="25">
+      <c r="C7" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="23">
         <v>43449</v>
       </c>
-      <c r="E7" s="26" t="s">
-        <v>36</v>
+      <c r="E7" s="24" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="37.5">
-      <c r="B8" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="25">
+      <c r="B8" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="23">
         <v>43467</v>
       </c>
-      <c r="E8" s="26" t="s">
-        <v>36</v>
+      <c r="E8" s="24" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="23"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="24"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="23"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="26"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24"/>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="23"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="23"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24"/>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="26"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="26"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="26"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="26"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="26"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24"/>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="26"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="26"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24"/>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="26"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="26"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="24"/>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="26"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="26"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="24"/>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="26"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="26"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="24"/>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="26"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="26"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="24"/>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="26"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="24"/>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="26"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="24"/>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="26"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="24"/>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="26"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="24"/>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="26"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
@@ -1414,19 +1419,19 @@
         <v>1</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="H5" s="17" t="s">
         <v>14</v>
@@ -1439,7 +1444,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>9</v>
@@ -1463,19 +1468,19 @@
         <v>2</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>58</v>
+        <v>53</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>54</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>21</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H7" s="17" t="s">
         <v>18</v>
@@ -1487,17 +1492,17 @@
         <v>2</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="22"/>
+      <c r="E8" s="27"/>
       <c r="F8" s="10" t="s">
         <v>21</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>17</v>
@@ -1509,19 +1514,19 @@
         <v>3</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="H9" s="14" t="s">
         <v>19</v>
@@ -1533,22 +1538,22 @@
         <v>4</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>45</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>49</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>21</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I10" s="14"/>
     </row>
@@ -1557,19 +1562,19 @@
         <v>5</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="H11" s="14" t="s">
         <v>20</v>
@@ -1581,19 +1586,19 @@
         <v>6</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>19</v>
@@ -1605,25 +1610,25 @@
         <v>7</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>19</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1632,11 +1637,12 @@
     <mergeCell ref="E7:E8"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"GET,POST,PUT,DELETE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>